<commit_message>
[modify] get talk theme search result list api
</commit_message>
<xml_diff>
--- a/20.開発/60.API/20.API仕様書/【eternal】API仕様書_Ref004_トークテーマ検索結果一覧取得.xlsx
+++ b/20.開発/60.API/20.API仕様書/【eternal】API仕様書_Ref004_トークテーマ検索結果一覧取得.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27729"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="27320" windowHeight="15360" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13880" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="表紙" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">レスポンス!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'概要(トークテーマ一覧取得)'!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">リクエスト!$A$1:$BV$18</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">レスポンス!$A$1:$BV$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">レスポンス!$A$1:$BV$19</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'概要(トークテーマ一覧取得)'!$A$1:$BV$18</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">表紙!$A$1:$AZ$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">変更履歴!$A$1:$F$26</definedName>
@@ -51,10 +51,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="99">
   <si>
     <t>Confidential</t>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>【変更履歴】</t>
@@ -64,14 +64,14 @@
     <rPh sb="3" eb="5">
       <t>リレキ</t>
     </rPh>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>版</t>
     <rPh sb="0" eb="1">
       <t>ハン</t>
     </rPh>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>変更内容</t>
@@ -81,7 +81,7 @@
     <rPh sb="2" eb="4">
       <t>ナイヨウ</t>
     </rPh>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>改訂日</t>
@@ -91,7 +91,7 @@
     <rPh sb="2" eb="3">
       <t>ビ</t>
     </rPh>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>改訂者</t>
@@ -101,7 +101,7 @@
     <rPh sb="2" eb="3">
       <t>シャ</t>
     </rPh>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>設計書名</t>
@@ -111,21 +111,21 @@
     <rPh sb="3" eb="4">
       <t>メイ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>作成日</t>
     <rPh sb="0" eb="3">
       <t>サクセイビ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>作成者</t>
     <rPh sb="0" eb="3">
       <t>サクセイシャ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>改訂日</t>
@@ -135,7 +135,7 @@
     <rPh sb="2" eb="3">
       <t>ビ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>改訂者</t>
@@ -145,36 +145,36 @@
     <rPh sb="2" eb="3">
       <t>シャ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>ID</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>備考</t>
     <rPh sb="0" eb="2">
       <t>ビコウ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>必須</t>
     <rPh sb="0" eb="2">
       <t>ヒッス</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>0.0.1</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>■ 概要</t>
     <rPh sb="2" eb="4">
       <t>ガイヨウ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>■使用画面</t>
@@ -184,18 +184,18 @@
     <rPh sb="3" eb="5">
       <t>ガメン</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>#</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>画面ID</t>
     <rPh sb="0" eb="2">
       <t>ガメン</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>画面名</t>
@@ -205,30 +205,30 @@
     <rPh sb="2" eb="3">
       <t>メイ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>■ リクエスト</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>■ エンドポイント</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>#</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>GET</t>
   </si>
   <si>
     <t>エンドポイント</t>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>HTTPメソッド</t>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>項目名(英名)</t>
@@ -241,7 +241,7 @@
     <rPh sb="4" eb="6">
       <t>エイメイ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>項目名(和名)</t>
@@ -254,49 +254,49 @@
     <rPh sb="4" eb="6">
       <t>ワメイ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Java型</t>
     <rPh sb="4" eb="5">
       <t>ガタ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>BigDecimal</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>String</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>List&lt;?&gt;</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>JSON型</t>
     <rPh sb="4" eb="5">
       <t>ガタ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>LocalDate</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>LocalDateTime</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Number</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>■ レスポンス</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>初版作成</t>
@@ -309,7 +309,7 @@
     <rPh sb="2" eb="4">
       <t>サクセイ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>・トークテーマの一覧を取得する</t>
@@ -319,7 +319,7 @@
     <rPh sb="11" eb="13">
       <t>シュトク</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>・取得するトークテーマ数、順番を指定可能</t>
@@ -338,25 +338,25 @@
     <rPh sb="18" eb="20">
       <t>カノウ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>count</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>order</t>
   </si>
   <si>
     <t>ソートキー</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>ソート順</t>
     <rPh sb="3" eb="4">
       <t>ジュン</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>取得数</t>
@@ -366,15 +366,15 @@
     <rPh sb="2" eb="3">
       <t>スウ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>sortKey</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>sortType</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>N</t>
@@ -384,27 +384,27 @@
   </si>
   <si>
     <t>・body</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>なし</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Number</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Boolean</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Array</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>String</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>rank:総合ランキング順
@@ -439,11 +439,11 @@
     <rPh sb="58" eb="60">
       <t>メイショウ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>maxCount</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>最大取得数</t>
@@ -456,7 +456,7 @@
     <rPh sb="4" eb="5">
       <t>スウ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>取得数の最大値</t>
@@ -469,19 +469,19 @@
     <rPh sb="4" eb="7">
       <t>サイダイチ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>BigDecimal</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>SortType</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>SortKeyType</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>asc:昇順
@@ -492,15 +492,12 @@
     <rPh sb="12" eb="14">
       <t>コウジュン</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>title</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>thumbnailUrl</t>
   </si>
   <si>
@@ -511,9 +508,6 @@
   </si>
   <si>
     <t>talkedCount</t>
-  </si>
-  <si>
-    <t>categoryList</t>
   </si>
   <si>
     <t>postedUser</t>
@@ -526,58 +520,36 @@
     <rPh sb="5" eb="6">
       <t>ジュン</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>トークテーマタイトル</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>トークテーマ概要</t>
-    <rPh sb="6" eb="8">
-      <t>ガイヨウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>サムネイルURL</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>GOOD数</t>
     <rPh sb="4" eb="5">
       <t>スウ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>BAD数</t>
     <rPh sb="3" eb="4">
       <t>スウ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>トーク数</t>
     <rPh sb="3" eb="4">
       <t>スウ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>カテゴリリスト</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>名称</t>
-    <rPh sb="0" eb="2">
-      <t>メイショウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>投稿日時</t>
@@ -587,11 +559,11 @@
     <rPh sb="2" eb="4">
       <t>ニチジ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>LocalDateTime</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>投稿者名</t>
@@ -601,42 +573,38 @@
     <rPh sb="3" eb="4">
       <t>メイ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>User</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>yyyyMMddHHmm形式</t>
     <rPh sb="12" eb="14">
       <t>ケイシキ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>talkTheme</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>トークテーマ</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>TalkTheme</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>List&lt;Category&gt;</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>・body</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>・クエリパラメータ</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>・以下の画面でAPIを使用する</t>
@@ -649,34 +617,26 @@
     <rPh sb="11" eb="13">
       <t>シヨウスル</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>talkThemeId</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>トークテーマID</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>カテゴリID</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>categoryId</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>searchWord</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>検索ワード</t>
     <rPh sb="0" eb="2">
       <t>ケンサク</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -688,7 +648,7 @@
         <color theme="1"/>
         <rFont val="メイリオ"/>
         <family val="2"/>
-        <charset val="128"/>
+        <charset val="129"/>
       </rPr>
       <t>serchT</t>
     </r>
@@ -697,34 +657,55 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
+        <family val="2"/>
+        <charset val="129"/>
       </rPr>
       <t>alklist</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>検索画面</t>
     <rPh sb="0" eb="2">
       <t>ケンサク</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Ref_004</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>中村</t>
     <rPh sb="0" eb="2">
       <t>ナカムラ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>HI-01-04</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>レスポンスからdescription削除、カテゴリリストを削除。</t>
+    <rPh sb="18" eb="20">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>サクジョ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>0.0.2</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>中村</t>
+    <rPh sb="0" eb="2">
+      <t>ナカムラ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
   </si>
 </sst>
 </file>
@@ -737,13 +718,20 @@
     <numFmt numFmtId="178" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
     <numFmt numFmtId="179" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Yu Gothic"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="メイリオ"/>
+      <family val="2"/>
+      <charset val="129"/>
     </font>
     <font>
       <sz val="12"/>
@@ -886,7 +874,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -989,17 +977,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -1029,205 +1006,178 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1">
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1277,7 +1227,7 @@
         <xdr:cNvPr id="3" name="グループ化 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1296,7 +1246,7 @@
           <xdr:cNvPr id="4" name="正方形/長方形 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1361,7 +1311,7 @@
           <xdr:cNvPr id="5" name="正方形/長方形 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1426,7 +1376,7 @@
           <xdr:cNvPr id="6" name="正方形/長方形 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1491,7 +1441,7 @@
           <xdr:cNvPr id="7" name="正方形/長方形 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1556,7 +1506,7 @@
           <xdr:cNvPr id="8" name="正方形/長方形 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1621,7 +1571,7 @@
           <xdr:cNvPr id="9" name="正方形/長方形 8">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000009000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1686,7 +1636,7 @@
           <xdr:cNvPr id="10" name="正方形/長方形 9">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000A000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1758,7 +1708,7 @@
           <xdr:cNvPr id="11" name="正方形/長方形 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000B000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1812,7 +1762,7 @@
                 <a:cs typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:pPr algn="ctr"/>
-              <a:t>【eternal】API仕様書_Ref001_トークテーマ一覧取得</a:t>
+              <a:t>【eternal】API仕様書_Ref004_トークテーマ検索結果一覧取得</a:t>
             </a:fld>
             <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
               <a:solidFill>
@@ -1830,7 +1780,7 @@
           <xdr:cNvPr id="12" name="正方形/長方形 11">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000C000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1902,7 +1852,7 @@
           <xdr:cNvPr id="13" name="正方形/長方形 12">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000D000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1974,7 +1924,7 @@
           <xdr:cNvPr id="14" name="正方形/長方形 13">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000E000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2046,7 +1996,7 @@
           <xdr:cNvPr id="15" name="正方形/長方形 14">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000F000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2139,7 +2089,7 @@
         <xdr:cNvPr id="2" name="グループ化 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F4161962-57F9-41FD-BE9B-9C39ABC6F599}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4161962-57F9-41FD-BE9B-9C39ABC6F599}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2158,7 +2108,7 @@
           <xdr:cNvPr id="3" name="正方形/長方形 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A8E14589-EE4C-491D-89A4-EB22863CB61C}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8E14589-EE4C-491D-89A4-EB22863CB61C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2223,7 +2173,7 @@
           <xdr:cNvPr id="4" name="正方形/長方形 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7A4FC26D-BF56-4446-B80D-0C5ACFEDC6A5}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A4FC26D-BF56-4446-B80D-0C5ACFEDC6A5}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2288,7 +2238,7 @@
           <xdr:cNvPr id="5" name="正方形/長方形 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{118AE21F-A33F-4231-A38E-5951C6EBB37D}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{118AE21F-A33F-4231-A38E-5951C6EBB37D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2353,7 +2303,7 @@
           <xdr:cNvPr id="6" name="正方形/長方形 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15CC184C-3B0C-4DA5-8121-88D86F00441F}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15CC184C-3B0C-4DA5-8121-88D86F00441F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2418,7 +2368,7 @@
           <xdr:cNvPr id="7" name="正方形/長方形 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4754AD5B-2B0B-46EE-8B71-66D219D5EC91}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4754AD5B-2B0B-46EE-8B71-66D219D5EC91}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2483,7 +2433,7 @@
           <xdr:cNvPr id="8" name="正方形/長方形 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0C0B29AA-73DD-4127-8070-ABBDAC015AE8}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C0B29AA-73DD-4127-8070-ABBDAC015AE8}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2548,7 +2498,7 @@
           <xdr:cNvPr id="9" name="正方形/長方形 8">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7E8159FD-54BB-4608-B580-BEF72FA5570A}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E8159FD-54BB-4608-B580-BEF72FA5570A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2620,7 +2570,7 @@
           <xdr:cNvPr id="10" name="正方形/長方形 9">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FB6D827E-0519-43AB-8D27-FC082F456CD0}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB6D827E-0519-43AB-8D27-FC082F456CD0}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2674,7 +2624,7 @@
                 <a:cs typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:pPr algn="ctr"/>
-              <a:t>【eternal】API仕様書_Ref001_トークテーマ一覧取得</a:t>
+              <a:t>【eternal】API仕様書_Ref004_トークテーマ検索結果一覧取得</a:t>
             </a:fld>
             <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
               <a:solidFill>
@@ -2692,7 +2642,7 @@
           <xdr:cNvPr id="11" name="正方形/長方形 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7C6F2712-88AD-4AB8-86C6-D7FB58A2F819}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C6F2712-88AD-4AB8-86C6-D7FB58A2F819}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2764,7 +2714,7 @@
           <xdr:cNvPr id="12" name="正方形/長方形 11">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15534BB0-4CA1-44E0-A343-8E7681B066C1}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15534BB0-4CA1-44E0-A343-8E7681B066C1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2836,7 +2786,7 @@
           <xdr:cNvPr id="13" name="正方形/長方形 12">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CFCA127E-94E6-429E-9CA3-34DA0CE0CE72}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFCA127E-94E6-429E-9CA3-34DA0CE0CE72}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2908,7 +2858,7 @@
           <xdr:cNvPr id="14" name="正方形/長方形 13">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{333B060A-0145-448A-A964-D699A9FE1714}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{333B060A-0145-448A-A964-D699A9FE1714}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3001,7 +2951,7 @@
         <xdr:cNvPr id="2" name="グループ化 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D26842C9-0618-40AE-B87D-E87EF0BA4636}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D26842C9-0618-40AE-B87D-E87EF0BA4636}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3020,7 +2970,7 @@
           <xdr:cNvPr id="3" name="正方形/長方形 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{67FBE5C9-53BB-4CF8-8AD1-EB095CBE281F}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67FBE5C9-53BB-4CF8-8AD1-EB095CBE281F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3085,7 +3035,7 @@
           <xdr:cNvPr id="4" name="正方形/長方形 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A6BA1B8A-20F1-46E8-94E5-10EC4AEE2D09}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6BA1B8A-20F1-46E8-94E5-10EC4AEE2D09}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3150,7 +3100,7 @@
           <xdr:cNvPr id="5" name="正方形/長方形 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9780BBE8-AC48-4FB7-AAE5-FCCABF1F3CAB}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9780BBE8-AC48-4FB7-AAE5-FCCABF1F3CAB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3215,7 +3165,7 @@
           <xdr:cNvPr id="6" name="正方形/長方形 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{75E881EB-BDAC-49DC-BC18-62C7AFFF07EB}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75E881EB-BDAC-49DC-BC18-62C7AFFF07EB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3280,7 +3230,7 @@
           <xdr:cNvPr id="7" name="正方形/長方形 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C8F811C6-71CA-4EB7-AA95-42C42BEC18E6}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8F811C6-71CA-4EB7-AA95-42C42BEC18E6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3345,7 +3295,7 @@
           <xdr:cNvPr id="8" name="正方形/長方形 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DFC81A55-158C-448F-BC49-95752FE3AC2A}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFC81A55-158C-448F-BC49-95752FE3AC2A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3410,7 +3360,7 @@
           <xdr:cNvPr id="9" name="正方形/長方形 8">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E94C7391-D5EA-46A1-90B1-7F7F94EB8CAE}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E94C7391-D5EA-46A1-90B1-7F7F94EB8CAE}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3482,7 +3432,7 @@
           <xdr:cNvPr id="10" name="正方形/長方形 9">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D45A86A5-E097-4C25-966B-43675226397A}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D45A86A5-E097-4C25-966B-43675226397A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3536,7 +3486,7 @@
                 <a:cs typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
               </a:rPr>
               <a:pPr algn="ctr"/>
-              <a:t>【eternal】API仕様書_Ref001_トークテーマ一覧取得</a:t>
+              <a:t>【eternal】API仕様書_Ref004_トークテーマ検索結果一覧取得</a:t>
             </a:fld>
             <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
               <a:solidFill>
@@ -3554,7 +3504,7 @@
           <xdr:cNvPr id="11" name="正方形/長方形 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15205912-C6AF-458D-B46C-B7B5D8916BEF}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15205912-C6AF-458D-B46C-B7B5D8916BEF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3626,7 +3576,7 @@
           <xdr:cNvPr id="12" name="正方形/長方形 11">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{08AB3292-595D-4F80-888F-88AA0A053D67}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08AB3292-595D-4F80-888F-88AA0A053D67}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3698,7 +3648,7 @@
           <xdr:cNvPr id="13" name="正方形/長方形 12">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E37098A9-4FA1-4543-9354-A3F5552B7C0F}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E37098A9-4FA1-4543-9354-A3F5552B7C0F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3770,7 +3720,7 @@
           <xdr:cNvPr id="14" name="正方形/長方形 13">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BD461C66-31E3-4F1F-A282-33FBF4E7E16F}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD461C66-31E3-4F1F-A282-33FBF4E7E16F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -4177,34 +4127,34 @@
     <row r="10" spans="1:26" ht="34">
       <c r="C10" s="3" t="str">
         <f ca="1">SUBSTITUTE(MID(CELL("filename",A1),FIND("[",CELL("filename",A1))+1,FIND("]",CELL("filename",A1))-FIND("[",CELL("filename",A1))-1),".xlsx","")</f>
-        <v>【eternal】API仕様書_Ref001_トークテーマ一覧取得</v>
+        <v>【eternal】API仕様書_Ref004_トークテーマ検索結果一覧取得</v>
       </c>
     </row>
     <row r="13" spans="1:26">
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="48"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="48"/>
-      <c r="O13" s="48"/>
-      <c r="P13" s="48"/>
-      <c r="Q13" s="48"/>
-      <c r="R13" s="48"/>
-      <c r="S13" s="48"/>
-      <c r="T13" s="48"/>
-      <c r="U13" s="48"/>
-      <c r="V13" s="48"/>
-      <c r="W13" s="48"/>
-      <c r="X13" s="48"/>
-      <c r="Y13" s="48"/>
-      <c r="Z13" s="48"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="41"/>
+      <c r="Y13" s="41"/>
+      <c r="Z13" s="41"/>
     </row>
     <row r="21" spans="2:51" ht="3" customHeight="1">
       <c r="B21" s="4"/>
@@ -4264,33 +4214,33 @@
       </c>
     </row>
     <row r="27" spans="2:51">
-      <c r="AO27" s="45">
+      <c r="AO27" s="38">
         <f ca="1">INDIRECT("変更履歴!"&amp;LEFT(ADDRESS(ROW(改訂日),COLUMN(改訂日),4,1),1)&amp;COUNTA(改訂日)+4)</f>
-        <v>43107</v>
-      </c>
-      <c r="AP27" s="46"/>
-      <c r="AQ27" s="46"/>
-      <c r="AR27" s="46"/>
-      <c r="AS27" s="46"/>
-      <c r="AT27" s="46"/>
-      <c r="AU27" s="46"/>
-      <c r="AV27" s="46"/>
-      <c r="AW27" s="46"/>
-      <c r="AX27" s="46"/>
-      <c r="AY27" s="46"/>
+        <v>43479</v>
+      </c>
+      <c r="AP27" s="39"/>
+      <c r="AQ27" s="39"/>
+      <c r="AR27" s="39"/>
+      <c r="AS27" s="39"/>
+      <c r="AT27" s="39"/>
+      <c r="AU27" s="39"/>
+      <c r="AV27" s="39"/>
+      <c r="AW27" s="39"/>
+      <c r="AX27" s="39"/>
+      <c r="AY27" s="39"/>
     </row>
     <row r="28" spans="2:51">
-      <c r="AR28" s="47" t="str">
+      <c r="AR28" s="40" t="str">
         <f ca="1">INDIRECT("変更履歴!"&amp;LEFT(ADDRESS(ROW(版),COLUMN(版),4,1),1)&amp;COUNTA(版)+4)</f>
-        <v>0.0.1</v>
-      </c>
-      <c r="AS28" s="47"/>
-      <c r="AT28" s="47"/>
-      <c r="AU28" s="47"/>
-      <c r="AV28" s="47"/>
-      <c r="AW28" s="47"/>
-      <c r="AX28" s="47"/>
-      <c r="AY28" s="47"/>
+        <v>0.0.2</v>
+      </c>
+      <c r="AS28" s="40"/>
+      <c r="AT28" s="40"/>
+      <c r="AU28" s="40"/>
+      <c r="AV28" s="40"/>
+      <c r="AW28" s="40"/>
+      <c r="AX28" s="40"/>
+      <c r="AY28" s="40"/>
     </row>
     <row r="31" spans="2:51">
       <c r="AR31" s="6"/>
@@ -4302,7 +4252,7 @@
     <mergeCell ref="AR28:AY28"/>
     <mergeCell ref="C13:Z13"/>
   </mergeCells>
-  <phoneticPr fontId="4"/>
+  <phoneticPr fontId="5"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="82" fitToWidth="0" orientation="landscape"/>
   <extLst>
@@ -4363,14 +4313,22 @@
         <v>43107</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="18"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="8"/>
+      <c r="B6" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="9">
+        <v>43479</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="18"/>
@@ -4487,7 +4445,7 @@
       <c r="E25" s="8"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4"/>
+  <phoneticPr fontId="5"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape"/>
   <extLst>
@@ -4505,7 +4463,7 @@
   </sheetPr>
   <dimension ref="A1:CC17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -4520,7 +4478,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:81" ht="6.75" customHeight="1">
-      <c r="A1" s="65"/>
+      <c r="A1" s="37"/>
     </row>
     <row r="2" spans="1:81">
       <c r="BX2" s="13" t="s">
@@ -4544,17 +4502,17 @@
     </row>
     <row r="3" spans="1:81">
       <c r="BX3" s="13" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="BY3" s="12" t="str">
         <f ca="1">REPLACE(LEFT(CELL("filename",$A$1),FIND(".x",CELL("filename",$A$1))-1),1,FIND("[",CELL("filename",$A$1)),)</f>
-        <v>【eternal】API仕様書_Ref001_トークテーマ一覧取得</v>
+        <v>【eternal】API仕様書_Ref004_トークテーマ検索結果一覧取得</v>
       </c>
       <c r="BZ3" s="14">
         <v>43107</v>
       </c>
       <c r="CA3" s="13" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="CB3" s="14"/>
       <c r="CC3" s="13"/>
@@ -4619,15 +4577,15 @@
       <c r="AH11" s="23"/>
     </row>
     <row r="12" spans="1:81" ht="19">
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="64" t="s">
-        <v>100</v>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="36" t="s">
+        <v>91</v>
       </c>
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
@@ -4663,7 +4621,7 @@
     </row>
     <row r="15" spans="1:81">
       <c r="C15" s="12" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:81">
@@ -4712,7 +4670,7 @@
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="19" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F17" s="20"/>
       <c r="G17" s="20"/>
@@ -4729,7 +4687,7 @@
       <c r="R17" s="20"/>
       <c r="S17" s="21"/>
       <c r="T17" s="20" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="U17" s="20"/>
       <c r="V17" s="20"/>
@@ -4750,7 +4708,7 @@
   <mergeCells count="1">
     <mergeCell ref="C12:G12"/>
   </mergeCells>
-  <phoneticPr fontId="4"/>
+  <phoneticPr fontId="5"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
       <formula1>"GET,POST,PUT,DELETE"</formula1>
@@ -4811,17 +4769,17 @@
     </row>
     <row r="3" spans="2:81">
       <c r="BX3" s="13" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="BY3" s="12" t="str">
         <f ca="1">REPLACE(LEFT(CELL("filename",$A$1),FIND(".x",CELL("filename",$A$1))-1),1,FIND("[",CELL("filename",$A$1)),)</f>
-        <v>【eternal】API仕様書_Ref001_トークテーマ一覧取得</v>
+        <v>【eternal】API仕様書_Ref004_トークテーマ検索結果一覧取得</v>
       </c>
       <c r="BZ3" s="14">
         <v>43107</v>
       </c>
       <c r="CA3" s="13" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="CB3" s="14"/>
       <c r="CC3" s="13"/>
@@ -4834,7 +4792,7 @@
     </row>
     <row r="7" spans="2:81">
       <c r="C7" s="12" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="BX7" s="12" t="s">
         <v>32</v>
@@ -4914,69 +4872,69 @@
       </c>
     </row>
     <row r="9" spans="2:81">
-      <c r="C9" s="54">
+      <c r="C9" s="48">
         <f>ROW()-ROW($C$8)</f>
         <v>1</v>
       </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54" t="s">
+      <c r="D9" s="48"/>
+      <c r="E9" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54" t="s">
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="M9" s="54"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="54"/>
-      <c r="P9" s="54"/>
-      <c r="Q9" s="54"/>
-      <c r="R9" s="54"/>
-      <c r="S9" s="54" t="s">
+      <c r="M9" s="48"/>
+      <c r="N9" s="48"/>
+      <c r="O9" s="48"/>
+      <c r="P9" s="48"/>
+      <c r="Q9" s="48"/>
+      <c r="R9" s="48"/>
+      <c r="S9" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="T9" s="54"/>
-      <c r="U9" s="54"/>
-      <c r="V9" s="54"/>
-      <c r="W9" s="54"/>
-      <c r="X9" s="54"/>
-      <c r="Y9" s="54"/>
-      <c r="Z9" s="54" t="s">
+      <c r="T9" s="48"/>
+      <c r="U9" s="48"/>
+      <c r="V9" s="48"/>
+      <c r="W9" s="48"/>
+      <c r="X9" s="48"/>
+      <c r="Y9" s="48"/>
+      <c r="Z9" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="AA9" s="54"/>
-      <c r="AB9" s="54"/>
-      <c r="AC9" s="54"/>
-      <c r="AD9" s="54"/>
-      <c r="AE9" s="54"/>
-      <c r="AF9" s="54"/>
-      <c r="AG9" s="52" t="s">
+      <c r="AA9" s="48"/>
+      <c r="AB9" s="48"/>
+      <c r="AC9" s="48"/>
+      <c r="AD9" s="48"/>
+      <c r="AE9" s="48"/>
+      <c r="AF9" s="48"/>
+      <c r="AG9" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="AH9" s="52"/>
-      <c r="AI9" s="53" t="s">
+      <c r="AH9" s="49"/>
+      <c r="AI9" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="AJ9" s="53"/>
-      <c r="AK9" s="53"/>
-      <c r="AL9" s="53"/>
-      <c r="AM9" s="53"/>
-      <c r="AN9" s="53"/>
-      <c r="AO9" s="53"/>
-      <c r="AP9" s="53"/>
-      <c r="AQ9" s="53"/>
-      <c r="AR9" s="53"/>
-      <c r="AS9" s="53"/>
-      <c r="AT9" s="53"/>
-      <c r="AU9" s="53"/>
-      <c r="AV9" s="53"/>
-      <c r="AW9" s="53"/>
-      <c r="AX9" s="53"/>
+      <c r="AJ9" s="50"/>
+      <c r="AK9" s="50"/>
+      <c r="AL9" s="50"/>
+      <c r="AM9" s="50"/>
+      <c r="AN9" s="50"/>
+      <c r="AO9" s="50"/>
+      <c r="AP9" s="50"/>
+      <c r="AQ9" s="50"/>
+      <c r="AR9" s="50"/>
+      <c r="AS9" s="50"/>
+      <c r="AT9" s="50"/>
+      <c r="AU9" s="50"/>
+      <c r="AV9" s="50"/>
+      <c r="AW9" s="50"/>
+      <c r="AX9" s="50"/>
       <c r="BX9" s="12" t="s">
         <v>30</v>
       </c>
@@ -4985,69 +4943,69 @@
       </c>
     </row>
     <row r="10" spans="2:81">
-      <c r="C10" s="54">
+      <c r="C10" s="48">
         <f>ROW()-ROW($C$8)</f>
         <v>2</v>
       </c>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54" t="s">
+      <c r="D10" s="48"/>
+      <c r="E10" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54" t="s">
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="M10" s="54"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="54"/>
-      <c r="P10" s="54"/>
-      <c r="Q10" s="54"/>
-      <c r="R10" s="54"/>
-      <c r="S10" s="54" t="s">
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="48"/>
+      <c r="R10" s="48"/>
+      <c r="S10" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="T10" s="54"/>
-      <c r="U10" s="54"/>
-      <c r="V10" s="54"/>
-      <c r="W10" s="54"/>
-      <c r="X10" s="54"/>
-      <c r="Y10" s="54"/>
-      <c r="Z10" s="54" t="s">
+      <c r="T10" s="48"/>
+      <c r="U10" s="48"/>
+      <c r="V10" s="48"/>
+      <c r="W10" s="48"/>
+      <c r="X10" s="48"/>
+      <c r="Y10" s="48"/>
+      <c r="Z10" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="AA10" s="54"/>
-      <c r="AB10" s="54"/>
-      <c r="AC10" s="54"/>
-      <c r="AD10" s="54"/>
-      <c r="AE10" s="54"/>
-      <c r="AF10" s="54"/>
-      <c r="AG10" s="52" t="s">
+      <c r="AA10" s="48"/>
+      <c r="AB10" s="48"/>
+      <c r="AC10" s="48"/>
+      <c r="AD10" s="48"/>
+      <c r="AE10" s="48"/>
+      <c r="AF10" s="48"/>
+      <c r="AG10" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="AH10" s="52"/>
-      <c r="AI10" s="53" t="s">
+      <c r="AH10" s="49"/>
+      <c r="AI10" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="AJ10" s="53"/>
-      <c r="AK10" s="53"/>
-      <c r="AL10" s="53"/>
-      <c r="AM10" s="53"/>
-      <c r="AN10" s="53"/>
-      <c r="AO10" s="53"/>
-      <c r="AP10" s="53"/>
-      <c r="AQ10" s="53"/>
-      <c r="AR10" s="53"/>
-      <c r="AS10" s="53"/>
-      <c r="AT10" s="53"/>
-      <c r="AU10" s="53"/>
-      <c r="AV10" s="53"/>
-      <c r="AW10" s="53"/>
-      <c r="AX10" s="53"/>
+      <c r="AJ10" s="50"/>
+      <c r="AK10" s="50"/>
+      <c r="AL10" s="50"/>
+      <c r="AM10" s="50"/>
+      <c r="AN10" s="50"/>
+      <c r="AO10" s="50"/>
+      <c r="AP10" s="50"/>
+      <c r="AQ10" s="50"/>
+      <c r="AR10" s="50"/>
+      <c r="AS10" s="50"/>
+      <c r="AT10" s="50"/>
+      <c r="AU10" s="50"/>
+      <c r="AV10" s="50"/>
+      <c r="AW10" s="50"/>
+      <c r="AX10" s="50"/>
       <c r="BX10" s="12" t="s">
         <v>52</v>
       </c>
@@ -5056,202 +5014,202 @@
       </c>
     </row>
     <row r="11" spans="2:81" ht="18" customHeight="1">
-      <c r="C11" s="61">
+      <c r="C11" s="45">
         <f>ROW()-ROW($C$8)</f>
         <v>3</v>
       </c>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61" t="s">
-        <v>98</v>
-      </c>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61" t="s">
-        <v>99</v>
-      </c>
-      <c r="M11" s="61"/>
-      <c r="N11" s="61"/>
-      <c r="O11" s="61"/>
-      <c r="P11" s="61"/>
-      <c r="Q11" s="61"/>
-      <c r="R11" s="61"/>
-      <c r="S11" s="61" t="s">
+      <c r="D11" s="45"/>
+      <c r="E11" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="M11" s="45"/>
+      <c r="N11" s="45"/>
+      <c r="O11" s="45"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="45"/>
+      <c r="R11" s="45"/>
+      <c r="S11" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="T11" s="61"/>
-      <c r="U11" s="61"/>
-      <c r="V11" s="61"/>
-      <c r="W11" s="61"/>
-      <c r="X11" s="61"/>
-      <c r="Y11" s="61"/>
-      <c r="Z11" s="61" t="s">
+      <c r="T11" s="45"/>
+      <c r="U11" s="45"/>
+      <c r="V11" s="45"/>
+      <c r="W11" s="45"/>
+      <c r="X11" s="45"/>
+      <c r="Y11" s="45"/>
+      <c r="Z11" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="AA11" s="61"/>
-      <c r="AB11" s="61"/>
-      <c r="AC11" s="61"/>
-      <c r="AD11" s="61"/>
-      <c r="AE11" s="61"/>
-      <c r="AF11" s="61"/>
-      <c r="AG11" s="62" t="s">
+      <c r="AA11" s="45"/>
+      <c r="AB11" s="45"/>
+      <c r="AC11" s="45"/>
+      <c r="AD11" s="45"/>
+      <c r="AE11" s="45"/>
+      <c r="AF11" s="45"/>
+      <c r="AG11" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="AH11" s="62"/>
-      <c r="AI11" s="63" t="s">
+      <c r="AH11" s="46"/>
+      <c r="AI11" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="AJ11" s="63"/>
-      <c r="AK11" s="63"/>
-      <c r="AL11" s="63"/>
-      <c r="AM11" s="63"/>
-      <c r="AN11" s="63"/>
-      <c r="AO11" s="63"/>
-      <c r="AP11" s="63"/>
-      <c r="AQ11" s="63"/>
-      <c r="AR11" s="63"/>
-      <c r="AS11" s="63"/>
-      <c r="AT11" s="63"/>
-      <c r="AU11" s="63"/>
-      <c r="AV11" s="63"/>
-      <c r="AW11" s="63"/>
-      <c r="AX11" s="63"/>
+      <c r="AJ11" s="47"/>
+      <c r="AK11" s="47"/>
+      <c r="AL11" s="47"/>
+      <c r="AM11" s="47"/>
+      <c r="AN11" s="47"/>
+      <c r="AO11" s="47"/>
+      <c r="AP11" s="47"/>
+      <c r="AQ11" s="47"/>
+      <c r="AR11" s="47"/>
+      <c r="AS11" s="47"/>
+      <c r="AT11" s="47"/>
+      <c r="AU11" s="47"/>
+      <c r="AV11" s="47"/>
+      <c r="AW11" s="47"/>
+      <c r="AX11" s="47"/>
     </row>
     <row r="12" spans="2:81" ht="95.25" customHeight="1">
-      <c r="C12" s="54">
+      <c r="C12" s="48">
         <f>ROW()-ROW($C$8)</f>
         <v>4</v>
       </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54" t="s">
+      <c r="D12" s="48"/>
+      <c r="E12" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="54" t="s">
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="M12" s="54"/>
-      <c r="N12" s="54"/>
-      <c r="O12" s="54"/>
-      <c r="P12" s="54"/>
-      <c r="Q12" s="54"/>
-      <c r="R12" s="54"/>
-      <c r="S12" s="54" t="s">
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="48"/>
+      <c r="S12" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="T12" s="54"/>
-      <c r="U12" s="54"/>
-      <c r="V12" s="54"/>
-      <c r="W12" s="54"/>
-      <c r="X12" s="54"/>
-      <c r="Y12" s="54"/>
-      <c r="Z12" s="54" t="s">
+      <c r="T12" s="48"/>
+      <c r="U12" s="48"/>
+      <c r="V12" s="48"/>
+      <c r="W12" s="48"/>
+      <c r="X12" s="48"/>
+      <c r="Y12" s="48"/>
+      <c r="Z12" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="AA12" s="54"/>
-      <c r="AB12" s="54"/>
-      <c r="AC12" s="54"/>
-      <c r="AD12" s="54"/>
-      <c r="AE12" s="54"/>
-      <c r="AF12" s="54"/>
-      <c r="AG12" s="52" t="s">
+      <c r="AA12" s="48"/>
+      <c r="AB12" s="48"/>
+      <c r="AC12" s="48"/>
+      <c r="AD12" s="48"/>
+      <c r="AE12" s="48"/>
+      <c r="AF12" s="48"/>
+      <c r="AG12" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="AH12" s="52"/>
-      <c r="AI12" s="53" t="s">
+      <c r="AH12" s="49"/>
+      <c r="AI12" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="AJ12" s="53"/>
-      <c r="AK12" s="53"/>
-      <c r="AL12" s="53"/>
-      <c r="AM12" s="53"/>
-      <c r="AN12" s="53"/>
-      <c r="AO12" s="53"/>
-      <c r="AP12" s="53"/>
-      <c r="AQ12" s="53"/>
-      <c r="AR12" s="53"/>
-      <c r="AS12" s="53"/>
-      <c r="AT12" s="53"/>
-      <c r="AU12" s="53"/>
-      <c r="AV12" s="53"/>
-      <c r="AW12" s="53"/>
-      <c r="AX12" s="53"/>
+      <c r="AJ12" s="50"/>
+      <c r="AK12" s="50"/>
+      <c r="AL12" s="50"/>
+      <c r="AM12" s="50"/>
+      <c r="AN12" s="50"/>
+      <c r="AO12" s="50"/>
+      <c r="AP12" s="50"/>
+      <c r="AQ12" s="50"/>
+      <c r="AR12" s="50"/>
+      <c r="AS12" s="50"/>
+      <c r="AT12" s="50"/>
+      <c r="AU12" s="50"/>
+      <c r="AV12" s="50"/>
+      <c r="AW12" s="50"/>
+      <c r="AX12" s="50"/>
       <c r="CA12" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="2:81" ht="38.25" customHeight="1">
-      <c r="C13" s="54">
+      <c r="C13" s="48">
         <f>ROW()-ROW($C$8)</f>
         <v>5</v>
       </c>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54" t="s">
+      <c r="D13" s="48"/>
+      <c r="E13" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="54" t="s">
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="M13" s="54"/>
-      <c r="N13" s="54"/>
-      <c r="O13" s="54"/>
-      <c r="P13" s="54"/>
-      <c r="Q13" s="54"/>
-      <c r="R13" s="54"/>
-      <c r="S13" s="54" t="s">
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="48"/>
+      <c r="P13" s="48"/>
+      <c r="Q13" s="48"/>
+      <c r="R13" s="48"/>
+      <c r="S13" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="T13" s="54"/>
-      <c r="U13" s="54"/>
-      <c r="V13" s="54"/>
-      <c r="W13" s="54"/>
-      <c r="X13" s="54"/>
-      <c r="Y13" s="54"/>
-      <c r="Z13" s="54" t="s">
+      <c r="T13" s="48"/>
+      <c r="U13" s="48"/>
+      <c r="V13" s="48"/>
+      <c r="W13" s="48"/>
+      <c r="X13" s="48"/>
+      <c r="Y13" s="48"/>
+      <c r="Z13" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="AA13" s="54"/>
-      <c r="AB13" s="54"/>
-      <c r="AC13" s="54"/>
-      <c r="AD13" s="54"/>
-      <c r="AE13" s="54"/>
-      <c r="AF13" s="54"/>
-      <c r="AG13" s="52" t="s">
+      <c r="AA13" s="48"/>
+      <c r="AB13" s="48"/>
+      <c r="AC13" s="48"/>
+      <c r="AD13" s="48"/>
+      <c r="AE13" s="48"/>
+      <c r="AF13" s="48"/>
+      <c r="AG13" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="AH13" s="52"/>
-      <c r="AI13" s="53" t="s">
+      <c r="AH13" s="49"/>
+      <c r="AI13" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="AJ13" s="53"/>
-      <c r="AK13" s="53"/>
-      <c r="AL13" s="53"/>
-      <c r="AM13" s="53"/>
-      <c r="AN13" s="53"/>
-      <c r="AO13" s="53"/>
-      <c r="AP13" s="53"/>
-      <c r="AQ13" s="53"/>
-      <c r="AR13" s="53"/>
-      <c r="AS13" s="53"/>
-      <c r="AT13" s="53"/>
-      <c r="AU13" s="53"/>
-      <c r="AV13" s="53"/>
-      <c r="AW13" s="53"/>
-      <c r="AX13" s="53"/>
+      <c r="AJ13" s="50"/>
+      <c r="AK13" s="50"/>
+      <c r="AL13" s="50"/>
+      <c r="AM13" s="50"/>
+      <c r="AN13" s="50"/>
+      <c r="AO13" s="50"/>
+      <c r="AP13" s="50"/>
+      <c r="AQ13" s="50"/>
+      <c r="AR13" s="50"/>
+      <c r="AS13" s="50"/>
+      <c r="AT13" s="50"/>
+      <c r="AU13" s="50"/>
+      <c r="AV13" s="50"/>
+      <c r="AW13" s="50"/>
+      <c r="AX13" s="50"/>
       <c r="CA13" s="12" t="s">
         <v>34</v>
       </c>
@@ -5326,70 +5284,74 @@
       <c r="AX16" s="23"/>
     </row>
     <row r="17" spans="3:50">
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="54"/>
-      <c r="O17" s="54"/>
-      <c r="P17" s="54"/>
-      <c r="Q17" s="54"/>
-      <c r="R17" s="54"/>
-      <c r="S17" s="54"/>
-      <c r="T17" s="54"/>
-      <c r="U17" s="54"/>
-      <c r="V17" s="54"/>
-      <c r="W17" s="54"/>
-      <c r="X17" s="54"/>
-      <c r="Y17" s="54"/>
-      <c r="Z17" s="54"/>
-      <c r="AA17" s="54"/>
-      <c r="AB17" s="54"/>
-      <c r="AC17" s="54"/>
-      <c r="AD17" s="54"/>
-      <c r="AE17" s="54"/>
-      <c r="AF17" s="54"/>
-      <c r="AG17" s="52"/>
-      <c r="AH17" s="52"/>
-      <c r="AI17" s="53"/>
-      <c r="AJ17" s="53"/>
-      <c r="AK17" s="53"/>
-      <c r="AL17" s="53"/>
-      <c r="AM17" s="53"/>
-      <c r="AN17" s="53"/>
-      <c r="AO17" s="53"/>
-      <c r="AP17" s="53"/>
-      <c r="AQ17" s="53"/>
-      <c r="AR17" s="53"/>
-      <c r="AS17" s="53"/>
-      <c r="AT17" s="53"/>
-      <c r="AU17" s="53"/>
-      <c r="AV17" s="53"/>
-      <c r="AW17" s="53"/>
-      <c r="AX17" s="53"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="48"/>
+      <c r="P17" s="48"/>
+      <c r="Q17" s="48"/>
+      <c r="R17" s="48"/>
+      <c r="S17" s="48"/>
+      <c r="T17" s="48"/>
+      <c r="U17" s="48"/>
+      <c r="V17" s="48"/>
+      <c r="W17" s="48"/>
+      <c r="X17" s="48"/>
+      <c r="Y17" s="48"/>
+      <c r="Z17" s="48"/>
+      <c r="AA17" s="48"/>
+      <c r="AB17" s="48"/>
+      <c r="AC17" s="48"/>
+      <c r="AD17" s="48"/>
+      <c r="AE17" s="48"/>
+      <c r="AF17" s="48"/>
+      <c r="AG17" s="49"/>
+      <c r="AH17" s="49"/>
+      <c r="AI17" s="50"/>
+      <c r="AJ17" s="50"/>
+      <c r="AK17" s="50"/>
+      <c r="AL17" s="50"/>
+      <c r="AM17" s="50"/>
+      <c r="AN17" s="50"/>
+      <c r="AO17" s="50"/>
+      <c r="AP17" s="50"/>
+      <c r="AQ17" s="50"/>
+      <c r="AR17" s="50"/>
+      <c r="AS17" s="50"/>
+      <c r="AT17" s="50"/>
+      <c r="AU17" s="50"/>
+      <c r="AV17" s="50"/>
+      <c r="AW17" s="50"/>
+      <c r="AX17" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:K11"/>
-    <mergeCell ref="L11:R11"/>
-    <mergeCell ref="S11:Y11"/>
-    <mergeCell ref="Z11:AF11"/>
-    <mergeCell ref="AG11:AH11"/>
-    <mergeCell ref="AI11:AX11"/>
-    <mergeCell ref="S9:Y9"/>
-    <mergeCell ref="Z9:AF9"/>
-    <mergeCell ref="AG9:AH9"/>
-    <mergeCell ref="AI9:AX9"/>
+    <mergeCell ref="E10:K10"/>
+    <mergeCell ref="L10:R10"/>
+    <mergeCell ref="S10:Y10"/>
+    <mergeCell ref="Z10:AF10"/>
+    <mergeCell ref="AG17:AH17"/>
+    <mergeCell ref="AI17:AX17"/>
+    <mergeCell ref="AG12:AH12"/>
+    <mergeCell ref="AI12:AX12"/>
+    <mergeCell ref="AG10:AH10"/>
+    <mergeCell ref="AI10:AX10"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:K17"/>
+    <mergeCell ref="L17:R17"/>
+    <mergeCell ref="S17:Y17"/>
+    <mergeCell ref="Z17:AF17"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:K9"/>
     <mergeCell ref="L9:R9"/>
@@ -5405,24 +5367,20 @@
     <mergeCell ref="L13:R13"/>
     <mergeCell ref="S13:Y13"/>
     <mergeCell ref="Z13:AF13"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:K17"/>
-    <mergeCell ref="L17:R17"/>
-    <mergeCell ref="S17:Y17"/>
-    <mergeCell ref="Z17:AF17"/>
-    <mergeCell ref="AG17:AH17"/>
-    <mergeCell ref="AI17:AX17"/>
-    <mergeCell ref="AG12:AH12"/>
-    <mergeCell ref="AI12:AX12"/>
-    <mergeCell ref="AG10:AH10"/>
-    <mergeCell ref="AI10:AX10"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:K10"/>
-    <mergeCell ref="L10:R10"/>
-    <mergeCell ref="S10:Y10"/>
-    <mergeCell ref="Z10:AF10"/>
+    <mergeCell ref="AG11:AH11"/>
+    <mergeCell ref="AI11:AX11"/>
+    <mergeCell ref="S9:Y9"/>
+    <mergeCell ref="Z9:AF9"/>
+    <mergeCell ref="AG9:AH9"/>
+    <mergeCell ref="AI9:AX9"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:K11"/>
+    <mergeCell ref="L11:R11"/>
+    <mergeCell ref="S11:Y11"/>
+    <mergeCell ref="Z11:AF11"/>
   </mergeCells>
-  <phoneticPr fontId="4"/>
+  <phoneticPr fontId="5"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG17:AH17 AG9:AH13">
       <formula1>"Y,N"</formula1>
@@ -5444,9 +5402,9 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:CC22"/>
+  <dimension ref="B1:CC18"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -5483,17 +5441,17 @@
     </row>
     <row r="3" spans="2:81">
       <c r="BX3" s="13" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="BY3" s="12" t="str">
         <f ca="1">REPLACE(LEFT(CELL("filename",$A$1),FIND(".x",CELL("filename",$A$1))-1),1,FIND("[",CELL("filename",$A$1)),)</f>
-        <v>【eternal】API仕様書_Ref001_トークテーマ一覧取得</v>
+        <v>【eternal】API仕様書_Ref004_トークテーマ検索結果一覧取得</v>
       </c>
       <c r="BZ3" s="14">
         <v>43107</v>
       </c>
       <c r="CA3" s="13" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="CB3" s="14"/>
       <c r="CC3" s="13"/>
@@ -5506,7 +5464,7 @@
     </row>
     <row r="7" spans="2:81">
       <c r="C7" s="12" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="BX7" s="12" t="s">
         <v>32</v>
@@ -5587,67 +5545,67 @@
       </c>
     </row>
     <row r="9" spans="2:81">
-      <c r="C9" s="34">
+      <c r="C9" s="31">
         <v>1</v>
       </c>
-      <c r="D9" s="44"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="57" t="s">
-        <v>87</v>
-      </c>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="59"/>
-      <c r="M9" s="60" t="s">
-        <v>88</v>
-      </c>
-      <c r="N9" s="60"/>
-      <c r="O9" s="60"/>
-      <c r="P9" s="60"/>
-      <c r="Q9" s="60"/>
-      <c r="R9" s="60"/>
-      <c r="S9" s="60"/>
-      <c r="T9" s="60" t="s">
+      <c r="D9" s="35"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="N9" s="54"/>
+      <c r="O9" s="54"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="54"/>
+      <c r="R9" s="54"/>
+      <c r="S9" s="54"/>
+      <c r="T9" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="U9" s="60"/>
-      <c r="V9" s="60"/>
-      <c r="W9" s="60"/>
-      <c r="X9" s="60"/>
-      <c r="Y9" s="60"/>
-      <c r="Z9" s="60"/>
-      <c r="AA9" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB9" s="60"/>
-      <c r="AC9" s="60"/>
-      <c r="AD9" s="60"/>
-      <c r="AE9" s="60"/>
-      <c r="AF9" s="60"/>
-      <c r="AG9" s="60"/>
+      <c r="U9" s="54"/>
+      <c r="V9" s="54"/>
+      <c r="W9" s="54"/>
+      <c r="X9" s="54"/>
+      <c r="Y9" s="54"/>
+      <c r="Z9" s="54"/>
+      <c r="AA9" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB9" s="54"/>
+      <c r="AC9" s="54"/>
+      <c r="AD9" s="54"/>
+      <c r="AE9" s="54"/>
+      <c r="AF9" s="54"/>
+      <c r="AG9" s="54"/>
       <c r="AH9" s="55" t="s">
         <v>48</v>
       </c>
       <c r="AI9" s="55"/>
-      <c r="AJ9" s="56"/>
-      <c r="AK9" s="56"/>
-      <c r="AL9" s="56"/>
-      <c r="AM9" s="56"/>
-      <c r="AN9" s="56"/>
-      <c r="AO9" s="56"/>
-      <c r="AP9" s="56"/>
-      <c r="AQ9" s="56"/>
-      <c r="AR9" s="56"/>
-      <c r="AS9" s="56"/>
-      <c r="AT9" s="56"/>
-      <c r="AU9" s="56"/>
-      <c r="AV9" s="56"/>
-      <c r="AW9" s="56"/>
-      <c r="AX9" s="56"/>
-      <c r="AY9" s="56"/>
+      <c r="AJ9" s="51"/>
+      <c r="AK9" s="51"/>
+      <c r="AL9" s="51"/>
+      <c r="AM9" s="51"/>
+      <c r="AN9" s="51"/>
+      <c r="AO9" s="51"/>
+      <c r="AP9" s="51"/>
+      <c r="AQ9" s="51"/>
+      <c r="AR9" s="51"/>
+      <c r="AS9" s="51"/>
+      <c r="AT9" s="51"/>
+      <c r="AU9" s="51"/>
+      <c r="AV9" s="51"/>
+      <c r="AW9" s="51"/>
+      <c r="AX9" s="51"/>
+      <c r="AY9" s="51"/>
       <c r="BX9" s="12" t="s">
         <v>30</v>
       </c>
@@ -5656,67 +5614,67 @@
       </c>
     </row>
     <row r="10" spans="2:81">
-      <c r="C10" s="35"/>
-      <c r="D10" s="42">
+      <c r="C10" s="32"/>
+      <c r="D10" s="34">
         <v>1</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="58" t="s">
-        <v>94</v>
-      </c>
-      <c r="G10" s="58"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="59"/>
-      <c r="M10" s="60" t="s">
-        <v>95</v>
-      </c>
-      <c r="N10" s="60"/>
-      <c r="O10" s="60"/>
-      <c r="P10" s="60"/>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="60"/>
-      <c r="S10" s="60"/>
-      <c r="T10" s="60" t="s">
+      <c r="E10" s="33"/>
+      <c r="F10" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="54"/>
+      <c r="T10" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="U10" s="60"/>
-      <c r="V10" s="60"/>
-      <c r="W10" s="60"/>
-      <c r="X10" s="60"/>
-      <c r="Y10" s="60"/>
-      <c r="Z10" s="60"/>
-      <c r="AA10" s="60" t="s">
+      <c r="U10" s="54"/>
+      <c r="V10" s="54"/>
+      <c r="W10" s="54"/>
+      <c r="X10" s="54"/>
+      <c r="Y10" s="54"/>
+      <c r="Z10" s="54"/>
+      <c r="AA10" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="AB10" s="60"/>
-      <c r="AC10" s="60"/>
-      <c r="AD10" s="60"/>
-      <c r="AE10" s="60"/>
-      <c r="AF10" s="60"/>
-      <c r="AG10" s="60"/>
+      <c r="AB10" s="54"/>
+      <c r="AC10" s="54"/>
+      <c r="AD10" s="54"/>
+      <c r="AE10" s="54"/>
+      <c r="AF10" s="54"/>
+      <c r="AG10" s="54"/>
       <c r="AH10" s="55" t="s">
         <v>48</v>
       </c>
       <c r="AI10" s="55"/>
-      <c r="AJ10" s="56"/>
-      <c r="AK10" s="56"/>
-      <c r="AL10" s="56"/>
-      <c r="AM10" s="56"/>
-      <c r="AN10" s="56"/>
-      <c r="AO10" s="56"/>
-      <c r="AP10" s="56"/>
-      <c r="AQ10" s="56"/>
-      <c r="AR10" s="56"/>
-      <c r="AS10" s="56"/>
-      <c r="AT10" s="56"/>
-      <c r="AU10" s="56"/>
-      <c r="AV10" s="56"/>
-      <c r="AW10" s="56"/>
-      <c r="AX10" s="56"/>
-      <c r="AY10" s="56"/>
+      <c r="AJ10" s="51"/>
+      <c r="AK10" s="51"/>
+      <c r="AL10" s="51"/>
+      <c r="AM10" s="51"/>
+      <c r="AN10" s="51"/>
+      <c r="AO10" s="51"/>
+      <c r="AP10" s="51"/>
+      <c r="AQ10" s="51"/>
+      <c r="AR10" s="51"/>
+      <c r="AS10" s="51"/>
+      <c r="AT10" s="51"/>
+      <c r="AU10" s="51"/>
+      <c r="AV10" s="51"/>
+      <c r="AW10" s="51"/>
+      <c r="AX10" s="51"/>
+      <c r="AY10" s="51"/>
       <c r="BX10" s="12" t="s">
         <v>52</v>
       </c>
@@ -5725,67 +5683,67 @@
       </c>
     </row>
     <row r="11" spans="2:81">
-      <c r="C11" s="35"/>
-      <c r="D11" s="42">
+      <c r="C11" s="32"/>
+      <c r="D11" s="34">
         <v>2</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="57" t="s">
+      <c r="E11" s="33"/>
+      <c r="F11" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="59"/>
-      <c r="M11" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="N11" s="60"/>
-      <c r="O11" s="60"/>
-      <c r="P11" s="60"/>
-      <c r="Q11" s="60"/>
-      <c r="R11" s="60"/>
-      <c r="S11" s="60"/>
-      <c r="T11" s="60" t="s">
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="54" t="s">
+        <v>70</v>
+      </c>
+      <c r="N11" s="54"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="54"/>
+      <c r="R11" s="54"/>
+      <c r="S11" s="54"/>
+      <c r="T11" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="U11" s="60"/>
-      <c r="V11" s="60"/>
-      <c r="W11" s="60"/>
-      <c r="X11" s="60"/>
-      <c r="Y11" s="60"/>
-      <c r="Z11" s="60"/>
-      <c r="AA11" s="60" t="s">
+      <c r="U11" s="54"/>
+      <c r="V11" s="54"/>
+      <c r="W11" s="54"/>
+      <c r="X11" s="54"/>
+      <c r="Y11" s="54"/>
+      <c r="Z11" s="54"/>
+      <c r="AA11" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="AB11" s="60"/>
-      <c r="AC11" s="60"/>
-      <c r="AD11" s="60"/>
-      <c r="AE11" s="60"/>
-      <c r="AF11" s="60"/>
-      <c r="AG11" s="60"/>
+      <c r="AB11" s="54"/>
+      <c r="AC11" s="54"/>
+      <c r="AD11" s="54"/>
+      <c r="AE11" s="54"/>
+      <c r="AF11" s="54"/>
+      <c r="AG11" s="54"/>
       <c r="AH11" s="55" t="s">
         <v>48</v>
       </c>
       <c r="AI11" s="55"/>
-      <c r="AJ11" s="56"/>
-      <c r="AK11" s="56"/>
-      <c r="AL11" s="56"/>
-      <c r="AM11" s="56"/>
-      <c r="AN11" s="56"/>
-      <c r="AO11" s="56"/>
-      <c r="AP11" s="56"/>
-      <c r="AQ11" s="56"/>
-      <c r="AR11" s="56"/>
-      <c r="AS11" s="56"/>
-      <c r="AT11" s="56"/>
-      <c r="AU11" s="56"/>
-      <c r="AV11" s="56"/>
-      <c r="AW11" s="56"/>
-      <c r="AX11" s="56"/>
-      <c r="AY11" s="56"/>
+      <c r="AJ11" s="51"/>
+      <c r="AK11" s="51"/>
+      <c r="AL11" s="51"/>
+      <c r="AM11" s="51"/>
+      <c r="AN11" s="51"/>
+      <c r="AO11" s="51"/>
+      <c r="AP11" s="51"/>
+      <c r="AQ11" s="51"/>
+      <c r="AR11" s="51"/>
+      <c r="AS11" s="51"/>
+      <c r="AT11" s="51"/>
+      <c r="AU11" s="51"/>
+      <c r="AV11" s="51"/>
+      <c r="AW11" s="51"/>
+      <c r="AX11" s="51"/>
+      <c r="AY11" s="51"/>
       <c r="BX11" s="12" t="s">
         <v>53</v>
       </c>
@@ -5794,719 +5752,495 @@
       </c>
     </row>
     <row r="12" spans="2:81">
-      <c r="C12" s="35"/>
-      <c r="D12" s="42">
+      <c r="C12" s="32"/>
+      <c r="D12" s="34">
         <v>3</v>
       </c>
-      <c r="E12" s="41"/>
-      <c r="F12" s="57" t="s">
+      <c r="E12" s="33"/>
+      <c r="F12" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="59"/>
-      <c r="M12" s="60" t="s">
-        <v>73</v>
-      </c>
-      <c r="N12" s="60"/>
-      <c r="O12" s="60"/>
-      <c r="P12" s="60"/>
-      <c r="Q12" s="60"/>
-      <c r="R12" s="60"/>
-      <c r="S12" s="60"/>
-      <c r="T12" s="60" t="s">
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="N12" s="54"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="54"/>
+      <c r="R12" s="54"/>
+      <c r="S12" s="54"/>
+      <c r="T12" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="U12" s="60"/>
-      <c r="V12" s="60"/>
-      <c r="W12" s="60"/>
-      <c r="X12" s="60"/>
-      <c r="Y12" s="60"/>
-      <c r="Z12" s="60"/>
-      <c r="AA12" s="60" t="s">
+      <c r="U12" s="54"/>
+      <c r="V12" s="54"/>
+      <c r="W12" s="54"/>
+      <c r="X12" s="54"/>
+      <c r="Y12" s="54"/>
+      <c r="Z12" s="54"/>
+      <c r="AA12" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="AB12" s="60"/>
-      <c r="AC12" s="60"/>
-      <c r="AD12" s="60"/>
-      <c r="AE12" s="60"/>
-      <c r="AF12" s="60"/>
-      <c r="AG12" s="60"/>
+      <c r="AB12" s="54"/>
+      <c r="AC12" s="54"/>
+      <c r="AD12" s="54"/>
+      <c r="AE12" s="54"/>
+      <c r="AF12" s="54"/>
+      <c r="AG12" s="54"/>
       <c r="AH12" s="55" t="s">
         <v>48</v>
       </c>
       <c r="AI12" s="55"/>
-      <c r="AJ12" s="56"/>
-      <c r="AK12" s="56"/>
-      <c r="AL12" s="56"/>
-      <c r="AM12" s="56"/>
-      <c r="AN12" s="56"/>
-      <c r="AO12" s="56"/>
-      <c r="AP12" s="56"/>
-      <c r="AQ12" s="56"/>
-      <c r="AR12" s="56"/>
-      <c r="AS12" s="56"/>
-      <c r="AT12" s="56"/>
-      <c r="AU12" s="56"/>
-      <c r="AV12" s="56"/>
-      <c r="AW12" s="56"/>
-      <c r="AX12" s="56"/>
-      <c r="AY12" s="56"/>
+      <c r="AJ12" s="51"/>
+      <c r="AK12" s="51"/>
+      <c r="AL12" s="51"/>
+      <c r="AM12" s="51"/>
+      <c r="AN12" s="51"/>
+      <c r="AO12" s="51"/>
+      <c r="AP12" s="51"/>
+      <c r="AQ12" s="51"/>
+      <c r="AR12" s="51"/>
+      <c r="AS12" s="51"/>
+      <c r="AT12" s="51"/>
+      <c r="AU12" s="51"/>
+      <c r="AV12" s="51"/>
+      <c r="AW12" s="51"/>
+      <c r="AX12" s="51"/>
+      <c r="AY12" s="51"/>
       <c r="CA12" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="2:81">
-      <c r="C13" s="35"/>
-      <c r="D13" s="42">
-        <v>4</v>
-      </c>
-      <c r="E13" s="41"/>
-      <c r="F13" s="57" t="s">
+      <c r="C13" s="32"/>
+      <c r="D13" s="34">
+        <v>5</v>
+      </c>
+      <c r="E13" s="33"/>
+      <c r="F13" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="60" t="s">
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="53"/>
+      <c r="M13" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="N13" s="54"/>
+      <c r="O13" s="54"/>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="54"/>
+      <c r="S13" s="54"/>
+      <c r="T13" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="U13" s="54"/>
+      <c r="V13" s="54"/>
+      <c r="W13" s="54"/>
+      <c r="X13" s="54"/>
+      <c r="Y13" s="54"/>
+      <c r="Z13" s="54"/>
+      <c r="AA13" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB13" s="54"/>
+      <c r="AC13" s="54"/>
+      <c r="AD13" s="54"/>
+      <c r="AE13" s="54"/>
+      <c r="AF13" s="54"/>
+      <c r="AG13" s="54"/>
+      <c r="AH13" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI13" s="55"/>
+      <c r="AJ13" s="51"/>
+      <c r="AK13" s="51"/>
+      <c r="AL13" s="51"/>
+      <c r="AM13" s="51"/>
+      <c r="AN13" s="51"/>
+      <c r="AO13" s="51"/>
+      <c r="AP13" s="51"/>
+      <c r="AQ13" s="51"/>
+      <c r="AR13" s="51"/>
+      <c r="AS13" s="51"/>
+      <c r="AT13" s="51"/>
+      <c r="AU13" s="51"/>
+      <c r="AV13" s="51"/>
+      <c r="AW13" s="51"/>
+      <c r="AX13" s="51"/>
+      <c r="AY13" s="51"/>
+    </row>
+    <row r="14" spans="2:81">
+      <c r="C14" s="32"/>
+      <c r="D14" s="34">
+        <v>6</v>
+      </c>
+      <c r="E14" s="33"/>
+      <c r="F14" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="N14" s="54"/>
+      <c r="O14" s="54"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="54"/>
+      <c r="R14" s="54"/>
+      <c r="S14" s="54"/>
+      <c r="T14" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="U14" s="54"/>
+      <c r="V14" s="54"/>
+      <c r="W14" s="54"/>
+      <c r="X14" s="54"/>
+      <c r="Y14" s="54"/>
+      <c r="Z14" s="54"/>
+      <c r="AA14" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB14" s="54"/>
+      <c r="AC14" s="54"/>
+      <c r="AD14" s="54"/>
+      <c r="AE14" s="54"/>
+      <c r="AF14" s="54"/>
+      <c r="AG14" s="54"/>
+      <c r="AH14" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI14" s="55"/>
+      <c r="AJ14" s="51"/>
+      <c r="AK14" s="51"/>
+      <c r="AL14" s="51"/>
+      <c r="AM14" s="51"/>
+      <c r="AN14" s="51"/>
+      <c r="AO14" s="51"/>
+      <c r="AP14" s="51"/>
+      <c r="AQ14" s="51"/>
+      <c r="AR14" s="51"/>
+      <c r="AS14" s="51"/>
+      <c r="AT14" s="51"/>
+      <c r="AU14" s="51"/>
+      <c r="AV14" s="51"/>
+      <c r="AW14" s="51"/>
+      <c r="AX14" s="51"/>
+      <c r="AY14" s="51"/>
+    </row>
+    <row r="15" spans="2:81">
+      <c r="C15" s="32"/>
+      <c r="D15" s="34">
+        <v>7</v>
+      </c>
+      <c r="E15" s="33"/>
+      <c r="F15" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="N13" s="60"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="60"/>
-      <c r="Q13" s="60"/>
-      <c r="R13" s="60"/>
-      <c r="S13" s="60"/>
-      <c r="T13" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="U13" s="60"/>
-      <c r="V13" s="60"/>
-      <c r="W13" s="60"/>
-      <c r="X13" s="60"/>
-      <c r="Y13" s="60"/>
-      <c r="Z13" s="60"/>
-      <c r="AA13" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB13" s="60"/>
-      <c r="AC13" s="60"/>
-      <c r="AD13" s="60"/>
-      <c r="AE13" s="60"/>
-      <c r="AF13" s="60"/>
-      <c r="AG13" s="60"/>
-      <c r="AH13" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI13" s="55"/>
-      <c r="AJ13" s="56"/>
-      <c r="AK13" s="56"/>
-      <c r="AL13" s="56"/>
-      <c r="AM13" s="56"/>
-      <c r="AN13" s="56"/>
-      <c r="AO13" s="56"/>
-      <c r="AP13" s="56"/>
-      <c r="AQ13" s="56"/>
-      <c r="AR13" s="56"/>
-      <c r="AS13" s="56"/>
-      <c r="AT13" s="56"/>
-      <c r="AU13" s="56"/>
-      <c r="AV13" s="56"/>
-      <c r="AW13" s="56"/>
-      <c r="AX13" s="56"/>
-      <c r="AY13" s="56"/>
-      <c r="CA13" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="2:81">
-      <c r="C14" s="35"/>
-      <c r="D14" s="42">
-        <v>5</v>
-      </c>
-      <c r="E14" s="41"/>
-      <c r="F14" s="57" t="s">
-        <v>65</v>
-      </c>
-      <c r="G14" s="58"/>
-      <c r="H14" s="58"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="58"/>
-      <c r="L14" s="59"/>
-      <c r="M14" s="60" t="s">
-        <v>75</v>
-      </c>
-      <c r="N14" s="60"/>
-      <c r="O14" s="60"/>
-      <c r="P14" s="60"/>
-      <c r="Q14" s="60"/>
-      <c r="R14" s="60"/>
-      <c r="S14" s="60"/>
-      <c r="T14" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="U14" s="60"/>
-      <c r="V14" s="60"/>
-      <c r="W14" s="60"/>
-      <c r="X14" s="60"/>
-      <c r="Y14" s="60"/>
-      <c r="Z14" s="60"/>
-      <c r="AA14" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB14" s="60"/>
-      <c r="AC14" s="60"/>
-      <c r="AD14" s="60"/>
-      <c r="AE14" s="60"/>
-      <c r="AF14" s="60"/>
-      <c r="AG14" s="60"/>
-      <c r="AH14" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI14" s="55"/>
-      <c r="AJ14" s="56"/>
-      <c r="AK14" s="56"/>
-      <c r="AL14" s="56"/>
-      <c r="AM14" s="56"/>
-      <c r="AN14" s="56"/>
-      <c r="AO14" s="56"/>
-      <c r="AP14" s="56"/>
-      <c r="AQ14" s="56"/>
-      <c r="AR14" s="56"/>
-      <c r="AS14" s="56"/>
-      <c r="AT14" s="56"/>
-      <c r="AU14" s="56"/>
-      <c r="AV14" s="56"/>
-      <c r="AW14" s="56"/>
-      <c r="AX14" s="56"/>
-      <c r="AY14" s="56"/>
-    </row>
-    <row r="15" spans="2:81">
-      <c r="C15" s="35"/>
-      <c r="D15" s="42">
-        <v>6</v>
-      </c>
-      <c r="E15" s="41"/>
-      <c r="F15" s="57" t="s">
-        <v>66</v>
-      </c>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="60" t="s">
-        <v>76</v>
-      </c>
-      <c r="N15" s="60"/>
-      <c r="O15" s="60"/>
-      <c r="P15" s="60"/>
-      <c r="Q15" s="60"/>
-      <c r="R15" s="60"/>
-      <c r="S15" s="60"/>
-      <c r="T15" s="60" t="s">
+      <c r="N15" s="54"/>
+      <c r="O15" s="54"/>
+      <c r="P15" s="54"/>
+      <c r="Q15" s="54"/>
+      <c r="R15" s="54"/>
+      <c r="S15" s="54"/>
+      <c r="T15" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="U15" s="60"/>
-      <c r="V15" s="60"/>
-      <c r="W15" s="60"/>
-      <c r="X15" s="60"/>
-      <c r="Y15" s="60"/>
-      <c r="Z15" s="60"/>
-      <c r="AA15" s="60" t="s">
+      <c r="U15" s="54"/>
+      <c r="V15" s="54"/>
+      <c r="W15" s="54"/>
+      <c r="X15" s="54"/>
+      <c r="Y15" s="54"/>
+      <c r="Z15" s="54"/>
+      <c r="AA15" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="AB15" s="60"/>
-      <c r="AC15" s="60"/>
-      <c r="AD15" s="60"/>
-      <c r="AE15" s="60"/>
-      <c r="AF15" s="60"/>
-      <c r="AG15" s="60"/>
+      <c r="AB15" s="54"/>
+      <c r="AC15" s="54"/>
+      <c r="AD15" s="54"/>
+      <c r="AE15" s="54"/>
+      <c r="AF15" s="54"/>
+      <c r="AG15" s="54"/>
       <c r="AH15" s="55" t="s">
         <v>48</v>
       </c>
       <c r="AI15" s="55"/>
-      <c r="AJ15" s="56"/>
-      <c r="AK15" s="56"/>
-      <c r="AL15" s="56"/>
-      <c r="AM15" s="56"/>
-      <c r="AN15" s="56"/>
-      <c r="AO15" s="56"/>
-      <c r="AP15" s="56"/>
-      <c r="AQ15" s="56"/>
-      <c r="AR15" s="56"/>
-      <c r="AS15" s="56"/>
-      <c r="AT15" s="56"/>
-      <c r="AU15" s="56"/>
-      <c r="AV15" s="56"/>
-      <c r="AW15" s="56"/>
-      <c r="AX15" s="56"/>
-      <c r="AY15" s="56"/>
+      <c r="AJ15" s="51"/>
+      <c r="AK15" s="51"/>
+      <c r="AL15" s="51"/>
+      <c r="AM15" s="51"/>
+      <c r="AN15" s="51"/>
+      <c r="AO15" s="51"/>
+      <c r="AP15" s="51"/>
+      <c r="AQ15" s="51"/>
+      <c r="AR15" s="51"/>
+      <c r="AS15" s="51"/>
+      <c r="AT15" s="51"/>
+      <c r="AU15" s="51"/>
+      <c r="AV15" s="51"/>
+      <c r="AW15" s="51"/>
+      <c r="AX15" s="51"/>
+      <c r="AY15" s="51"/>
     </row>
     <row r="16" spans="2:81">
-      <c r="C16" s="35"/>
-      <c r="D16" s="42">
-        <v>7</v>
-      </c>
-      <c r="E16" s="41"/>
-      <c r="F16" s="57" t="s">
+      <c r="C16" s="32"/>
+      <c r="D16" s="34">
+        <v>8</v>
+      </c>
+      <c r="E16" s="33"/>
+      <c r="F16" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="58"/>
-      <c r="K16" s="58"/>
-      <c r="L16" s="59"/>
-      <c r="M16" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="N16" s="60"/>
-      <c r="O16" s="60"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="60"/>
-      <c r="R16" s="60"/>
-      <c r="S16" s="60"/>
-      <c r="T16" s="60" t="s">
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="N16" s="54"/>
+      <c r="O16" s="54"/>
+      <c r="P16" s="54"/>
+      <c r="Q16" s="54"/>
+      <c r="R16" s="54"/>
+      <c r="S16" s="54"/>
+      <c r="T16" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="U16" s="60"/>
-      <c r="V16" s="60"/>
-      <c r="W16" s="60"/>
-      <c r="X16" s="60"/>
-      <c r="Y16" s="60"/>
-      <c r="Z16" s="60"/>
-      <c r="AA16" s="60" t="s">
+      <c r="U16" s="54"/>
+      <c r="V16" s="54"/>
+      <c r="W16" s="54"/>
+      <c r="X16" s="54"/>
+      <c r="Y16" s="54"/>
+      <c r="Z16" s="54"/>
+      <c r="AA16" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="AB16" s="60"/>
-      <c r="AC16" s="60"/>
-      <c r="AD16" s="60"/>
-      <c r="AE16" s="60"/>
-      <c r="AF16" s="60"/>
-      <c r="AG16" s="60"/>
+      <c r="AB16" s="54"/>
+      <c r="AC16" s="54"/>
+      <c r="AD16" s="54"/>
+      <c r="AE16" s="54"/>
+      <c r="AF16" s="54"/>
+      <c r="AG16" s="54"/>
       <c r="AH16" s="55" t="s">
         <v>48</v>
       </c>
       <c r="AI16" s="55"/>
-      <c r="AJ16" s="56"/>
-      <c r="AK16" s="56"/>
-      <c r="AL16" s="56"/>
-      <c r="AM16" s="56"/>
-      <c r="AN16" s="56"/>
-      <c r="AO16" s="56"/>
-      <c r="AP16" s="56"/>
-      <c r="AQ16" s="56"/>
-      <c r="AR16" s="56"/>
-      <c r="AS16" s="56"/>
-      <c r="AT16" s="56"/>
-      <c r="AU16" s="56"/>
-      <c r="AV16" s="56"/>
-      <c r="AW16" s="56"/>
-      <c r="AX16" s="56"/>
-      <c r="AY16" s="56"/>
+      <c r="AJ16" s="51"/>
+      <c r="AK16" s="51"/>
+      <c r="AL16" s="51"/>
+      <c r="AM16" s="51"/>
+      <c r="AN16" s="51"/>
+      <c r="AO16" s="51"/>
+      <c r="AP16" s="51"/>
+      <c r="AQ16" s="51"/>
+      <c r="AR16" s="51"/>
+      <c r="AS16" s="51"/>
+      <c r="AT16" s="51"/>
+      <c r="AU16" s="51"/>
+      <c r="AV16" s="51"/>
+      <c r="AW16" s="51"/>
+      <c r="AX16" s="51"/>
+      <c r="AY16" s="51"/>
     </row>
     <row r="17" spans="3:51">
-      <c r="C17" s="35"/>
-      <c r="D17" s="31">
-        <v>8</v>
-      </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="57" t="s">
+      <c r="C17" s="32"/>
+      <c r="D17" s="29">
+        <v>9</v>
+      </c>
+      <c r="E17" s="30"/>
+      <c r="F17" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="58"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="60" t="s">
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="N17" s="60"/>
-      <c r="O17" s="60"/>
-      <c r="P17" s="60"/>
-      <c r="Q17" s="60"/>
-      <c r="R17" s="60"/>
-      <c r="S17" s="60"/>
-      <c r="T17" s="60" t="s">
-        <v>51</v>
-      </c>
-      <c r="U17" s="60"/>
-      <c r="V17" s="60"/>
-      <c r="W17" s="60"/>
-      <c r="X17" s="60"/>
-      <c r="Y17" s="60"/>
-      <c r="Z17" s="60"/>
-      <c r="AA17" s="60" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB17" s="60"/>
-      <c r="AC17" s="60"/>
-      <c r="AD17" s="60"/>
-      <c r="AE17" s="60"/>
-      <c r="AF17" s="60"/>
-      <c r="AG17" s="60"/>
+      <c r="N17" s="54"/>
+      <c r="O17" s="54"/>
+      <c r="P17" s="54"/>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="54"/>
+      <c r="S17" s="54"/>
+      <c r="T17" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="U17" s="54"/>
+      <c r="V17" s="54"/>
+      <c r="W17" s="54"/>
+      <c r="X17" s="54"/>
+      <c r="Y17" s="54"/>
+      <c r="Z17" s="54"/>
+      <c r="AA17" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB17" s="54"/>
+      <c r="AC17" s="54"/>
+      <c r="AD17" s="54"/>
+      <c r="AE17" s="54"/>
+      <c r="AF17" s="54"/>
+      <c r="AG17" s="54"/>
       <c r="AH17" s="55" t="s">
         <v>48</v>
       </c>
       <c r="AI17" s="55"/>
-      <c r="AJ17" s="56"/>
-      <c r="AK17" s="56"/>
-      <c r="AL17" s="56"/>
-      <c r="AM17" s="56"/>
-      <c r="AN17" s="56"/>
-      <c r="AO17" s="56"/>
-      <c r="AP17" s="56"/>
-      <c r="AQ17" s="56"/>
-      <c r="AR17" s="56"/>
-      <c r="AS17" s="56"/>
-      <c r="AT17" s="56"/>
-      <c r="AU17" s="56"/>
-      <c r="AV17" s="56"/>
-      <c r="AW17" s="56"/>
-      <c r="AX17" s="56"/>
-      <c r="AY17" s="56"/>
+      <c r="AJ17" s="51"/>
+      <c r="AK17" s="51"/>
+      <c r="AL17" s="51"/>
+      <c r="AM17" s="51"/>
+      <c r="AN17" s="51"/>
+      <c r="AO17" s="51"/>
+      <c r="AP17" s="51"/>
+      <c r="AQ17" s="51"/>
+      <c r="AR17" s="51"/>
+      <c r="AS17" s="51"/>
+      <c r="AT17" s="51"/>
+      <c r="AU17" s="51"/>
+      <c r="AV17" s="51"/>
+      <c r="AW17" s="51"/>
+      <c r="AX17" s="51"/>
+      <c r="AY17" s="51"/>
     </row>
     <row r="18" spans="3:51">
-      <c r="C18" s="43"/>
-      <c r="D18" s="37">
-        <v>9</v>
-      </c>
-      <c r="E18" s="38"/>
-      <c r="F18" s="58" t="s">
+      <c r="C18" s="15"/>
+      <c r="D18" s="34">
+        <v>10</v>
+      </c>
+      <c r="E18" s="33"/>
+      <c r="F18" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="G18" s="58"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="58"/>
-      <c r="K18" s="58"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="60" t="s">
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="53"/>
+      <c r="M18" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="N18" s="54"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="54"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="54"/>
+      <c r="S18" s="54"/>
+      <c r="T18" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="U18" s="54"/>
+      <c r="V18" s="54"/>
+      <c r="W18" s="54"/>
+      <c r="X18" s="54"/>
+      <c r="Y18" s="54"/>
+      <c r="Z18" s="54"/>
+      <c r="AA18" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB18" s="54"/>
+      <c r="AC18" s="54"/>
+      <c r="AD18" s="54"/>
+      <c r="AE18" s="54"/>
+      <c r="AF18" s="54"/>
+      <c r="AG18" s="54"/>
+      <c r="AH18" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI18" s="55"/>
+      <c r="AJ18" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="N18" s="60"/>
-      <c r="O18" s="60"/>
-      <c r="P18" s="60"/>
-      <c r="Q18" s="60"/>
-      <c r="R18" s="60"/>
-      <c r="S18" s="60"/>
-      <c r="T18" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="U18" s="60"/>
-      <c r="V18" s="60"/>
-      <c r="W18" s="60"/>
-      <c r="X18" s="60"/>
-      <c r="Y18" s="60"/>
-      <c r="Z18" s="60"/>
-      <c r="AA18" s="60" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB18" s="60"/>
-      <c r="AC18" s="60"/>
-      <c r="AD18" s="60"/>
-      <c r="AE18" s="60"/>
-      <c r="AF18" s="60"/>
-      <c r="AG18" s="60"/>
-      <c r="AH18" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI18" s="55"/>
-      <c r="AJ18" s="56"/>
-      <c r="AK18" s="56"/>
-      <c r="AL18" s="56"/>
-      <c r="AM18" s="56"/>
-      <c r="AN18" s="56"/>
-      <c r="AO18" s="56"/>
-      <c r="AP18" s="56"/>
-      <c r="AQ18" s="56"/>
-      <c r="AR18" s="56"/>
-      <c r="AS18" s="56"/>
-      <c r="AT18" s="56"/>
-      <c r="AU18" s="56"/>
-      <c r="AV18" s="56"/>
-      <c r="AW18" s="56"/>
-      <c r="AX18" s="56"/>
-      <c r="AY18" s="56"/>
-    </row>
-    <row r="19" spans="3:51">
-      <c r="C19" s="33"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="36">
-        <v>1</v>
-      </c>
-      <c r="F19" s="58" t="s">
-        <v>97</v>
-      </c>
-      <c r="G19" s="58"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="58"/>
-      <c r="K19" s="58"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="60" t="s">
-        <v>96</v>
-      </c>
-      <c r="N19" s="60"/>
-      <c r="O19" s="60"/>
-      <c r="P19" s="60"/>
-      <c r="Q19" s="60"/>
-      <c r="R19" s="60"/>
-      <c r="S19" s="60"/>
-      <c r="T19" s="60" t="s">
-        <v>51</v>
-      </c>
-      <c r="U19" s="60"/>
-      <c r="V19" s="60"/>
-      <c r="W19" s="60"/>
-      <c r="X19" s="60"/>
-      <c r="Y19" s="60"/>
-      <c r="Z19" s="60"/>
-      <c r="AA19" s="60" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB19" s="60"/>
-      <c r="AC19" s="60"/>
-      <c r="AD19" s="60"/>
-      <c r="AE19" s="60"/>
-      <c r="AF19" s="60"/>
-      <c r="AG19" s="60"/>
-      <c r="AH19" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI19" s="55"/>
-      <c r="AJ19" s="56"/>
-      <c r="AK19" s="56"/>
-      <c r="AL19" s="56"/>
-      <c r="AM19" s="56"/>
-      <c r="AN19" s="56"/>
-      <c r="AO19" s="56"/>
-      <c r="AP19" s="56"/>
-      <c r="AQ19" s="56"/>
-      <c r="AR19" s="56"/>
-      <c r="AS19" s="56"/>
-      <c r="AT19" s="56"/>
-      <c r="AU19" s="56"/>
-      <c r="AV19" s="56"/>
-      <c r="AW19" s="56"/>
-      <c r="AX19" s="56"/>
-      <c r="AY19" s="56"/>
-    </row>
-    <row r="20" spans="3:51">
-      <c r="C20" s="33"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="36">
-        <v>2</v>
-      </c>
-      <c r="F20" s="58" t="s">
-        <v>79</v>
-      </c>
-      <c r="G20" s="58"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
-      <c r="K20" s="58"/>
-      <c r="L20" s="59"/>
-      <c r="M20" s="60" t="s">
-        <v>81</v>
-      </c>
-      <c r="N20" s="60"/>
-      <c r="O20" s="60"/>
-      <c r="P20" s="60"/>
-      <c r="Q20" s="60"/>
-      <c r="R20" s="60"/>
-      <c r="S20" s="60"/>
-      <c r="T20" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="U20" s="60"/>
-      <c r="V20" s="60"/>
-      <c r="W20" s="60"/>
-      <c r="X20" s="60"/>
-      <c r="Y20" s="60"/>
-      <c r="Z20" s="60"/>
-      <c r="AA20" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB20" s="60"/>
-      <c r="AC20" s="60"/>
-      <c r="AD20" s="60"/>
-      <c r="AE20" s="60"/>
-      <c r="AF20" s="60"/>
-      <c r="AG20" s="60"/>
-      <c r="AH20" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI20" s="55"/>
-      <c r="AJ20" s="56"/>
-      <c r="AK20" s="56"/>
-      <c r="AL20" s="56"/>
-      <c r="AM20" s="56"/>
-      <c r="AN20" s="56"/>
-      <c r="AO20" s="56"/>
-      <c r="AP20" s="56"/>
-      <c r="AQ20" s="56"/>
-      <c r="AR20" s="56"/>
-      <c r="AS20" s="56"/>
-      <c r="AT20" s="56"/>
-      <c r="AU20" s="56"/>
-      <c r="AV20" s="56"/>
-      <c r="AW20" s="56"/>
-      <c r="AX20" s="56"/>
-      <c r="AY20" s="56"/>
-    </row>
-    <row r="21" spans="3:51">
-      <c r="C21" s="35"/>
-      <c r="D21" s="29">
-        <v>10</v>
-      </c>
-      <c r="E21" s="30"/>
-      <c r="F21" s="57" t="s">
-        <v>70</v>
-      </c>
-      <c r="G21" s="58"/>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="58"/>
-      <c r="L21" s="59"/>
-      <c r="M21" s="60" t="s">
-        <v>84</v>
-      </c>
-      <c r="N21" s="60"/>
-      <c r="O21" s="60"/>
-      <c r="P21" s="60"/>
-      <c r="Q21" s="60"/>
-      <c r="R21" s="60"/>
-      <c r="S21" s="60"/>
-      <c r="T21" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="U21" s="60"/>
-      <c r="V21" s="60"/>
-      <c r="W21" s="60"/>
-      <c r="X21" s="60"/>
-      <c r="Y21" s="60"/>
-      <c r="Z21" s="60"/>
-      <c r="AA21" s="60" t="s">
-        <v>85</v>
-      </c>
-      <c r="AB21" s="60"/>
-      <c r="AC21" s="60"/>
-      <c r="AD21" s="60"/>
-      <c r="AE21" s="60"/>
-      <c r="AF21" s="60"/>
-      <c r="AG21" s="60"/>
-      <c r="AH21" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI21" s="55"/>
-      <c r="AJ21" s="56"/>
-      <c r="AK21" s="56"/>
-      <c r="AL21" s="56"/>
-      <c r="AM21" s="56"/>
-      <c r="AN21" s="56"/>
-      <c r="AO21" s="56"/>
-      <c r="AP21" s="56"/>
-      <c r="AQ21" s="56"/>
-      <c r="AR21" s="56"/>
-      <c r="AS21" s="56"/>
-      <c r="AT21" s="56"/>
-      <c r="AU21" s="56"/>
-      <c r="AV21" s="56"/>
-      <c r="AW21" s="56"/>
-      <c r="AX21" s="56"/>
-      <c r="AY21" s="56"/>
-    </row>
-    <row r="22" spans="3:51">
-      <c r="C22" s="15"/>
-      <c r="D22" s="42">
-        <v>11</v>
-      </c>
-      <c r="E22" s="41"/>
-      <c r="F22" s="57" t="s">
-        <v>71</v>
-      </c>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="58"/>
-      <c r="K22" s="58"/>
-      <c r="L22" s="59"/>
-      <c r="M22" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="N22" s="60"/>
-      <c r="O22" s="60"/>
-      <c r="P22" s="60"/>
-      <c r="Q22" s="60"/>
-      <c r="R22" s="60"/>
-      <c r="S22" s="60"/>
-      <c r="T22" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="U22" s="60"/>
-      <c r="V22" s="60"/>
-      <c r="W22" s="60"/>
-      <c r="X22" s="60"/>
-      <c r="Y22" s="60"/>
-      <c r="Z22" s="60"/>
-      <c r="AA22" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB22" s="60"/>
-      <c r="AC22" s="60"/>
-      <c r="AD22" s="60"/>
-      <c r="AE22" s="60"/>
-      <c r="AF22" s="60"/>
-      <c r="AG22" s="60"/>
-      <c r="AH22" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI22" s="55"/>
-      <c r="AJ22" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="AK22" s="56"/>
-      <c r="AL22" s="56"/>
-      <c r="AM22" s="56"/>
-      <c r="AN22" s="56"/>
-      <c r="AO22" s="56"/>
-      <c r="AP22" s="56"/>
-      <c r="AQ22" s="56"/>
-      <c r="AR22" s="56"/>
-      <c r="AS22" s="56"/>
-      <c r="AT22" s="56"/>
-      <c r="AU22" s="56"/>
-      <c r="AV22" s="56"/>
-      <c r="AW22" s="56"/>
-      <c r="AX22" s="56"/>
-      <c r="AY22" s="56"/>
+      <c r="AK18" s="51"/>
+      <c r="AL18" s="51"/>
+      <c r="AM18" s="51"/>
+      <c r="AN18" s="51"/>
+      <c r="AO18" s="51"/>
+      <c r="AP18" s="51"/>
+      <c r="AQ18" s="51"/>
+      <c r="AR18" s="51"/>
+      <c r="AS18" s="51"/>
+      <c r="AT18" s="51"/>
+      <c r="AU18" s="51"/>
+      <c r="AV18" s="51"/>
+      <c r="AW18" s="51"/>
+      <c r="AX18" s="51"/>
+      <c r="AY18" s="51"/>
     </row>
   </sheetData>
-  <mergeCells count="84">
-    <mergeCell ref="AJ10:AY10"/>
-    <mergeCell ref="F10:L10"/>
-    <mergeCell ref="M10:S10"/>
-    <mergeCell ref="T10:Z10"/>
-    <mergeCell ref="AA10:AG10"/>
-    <mergeCell ref="AH10:AI10"/>
-    <mergeCell ref="F11:L11"/>
-    <mergeCell ref="F12:L12"/>
-    <mergeCell ref="M11:S11"/>
-    <mergeCell ref="T11:Z11"/>
-    <mergeCell ref="AA11:AG11"/>
+  <mergeCells count="60">
+    <mergeCell ref="AH9:AI9"/>
+    <mergeCell ref="AJ9:AY9"/>
+    <mergeCell ref="F9:L9"/>
+    <mergeCell ref="M9:S9"/>
+    <mergeCell ref="T9:Z9"/>
+    <mergeCell ref="AA9:AG9"/>
+    <mergeCell ref="AJ17:AY17"/>
+    <mergeCell ref="M18:S18"/>
+    <mergeCell ref="T18:Z18"/>
+    <mergeCell ref="AA18:AG18"/>
+    <mergeCell ref="AH18:AI18"/>
+    <mergeCell ref="AJ18:AY18"/>
+    <mergeCell ref="M17:S17"/>
+    <mergeCell ref="T17:Z17"/>
+    <mergeCell ref="AA17:AG17"/>
+    <mergeCell ref="AH17:AI17"/>
+    <mergeCell ref="F17:L17"/>
+    <mergeCell ref="F18:L18"/>
+    <mergeCell ref="AJ16:AY16"/>
+    <mergeCell ref="AH16:AI16"/>
+    <mergeCell ref="F16:L16"/>
+    <mergeCell ref="M16:S16"/>
+    <mergeCell ref="T16:Z16"/>
+    <mergeCell ref="AA16:AG16"/>
+    <mergeCell ref="AJ14:AY14"/>
+    <mergeCell ref="M15:S15"/>
+    <mergeCell ref="T15:Z15"/>
+    <mergeCell ref="AA15:AG15"/>
+    <mergeCell ref="AH15:AI15"/>
+    <mergeCell ref="AJ15:AY15"/>
+    <mergeCell ref="AH14:AI14"/>
+    <mergeCell ref="F14:L14"/>
+    <mergeCell ref="F15:L15"/>
+    <mergeCell ref="M14:S14"/>
+    <mergeCell ref="T14:Z14"/>
+    <mergeCell ref="AA14:AG14"/>
+    <mergeCell ref="M13:S13"/>
+    <mergeCell ref="T13:Z13"/>
+    <mergeCell ref="AA13:AG13"/>
+    <mergeCell ref="AH13:AI13"/>
+    <mergeCell ref="AJ13:AY13"/>
+    <mergeCell ref="F13:L13"/>
     <mergeCell ref="AJ11:AY11"/>
     <mergeCell ref="M12:S12"/>
     <mergeCell ref="T12:Z12"/>
@@ -6514,76 +6248,21 @@
     <mergeCell ref="AH12:AI12"/>
     <mergeCell ref="AJ12:AY12"/>
     <mergeCell ref="AH11:AI11"/>
-    <mergeCell ref="F13:L13"/>
-    <mergeCell ref="F14:L14"/>
-    <mergeCell ref="M13:S13"/>
-    <mergeCell ref="T13:Z13"/>
-    <mergeCell ref="AA13:AG13"/>
-    <mergeCell ref="AJ13:AY13"/>
-    <mergeCell ref="M14:S14"/>
-    <mergeCell ref="T14:Z14"/>
-    <mergeCell ref="AA14:AG14"/>
-    <mergeCell ref="AH14:AI14"/>
-    <mergeCell ref="AJ14:AY14"/>
-    <mergeCell ref="AH13:AI13"/>
-    <mergeCell ref="F15:L15"/>
-    <mergeCell ref="F16:L16"/>
-    <mergeCell ref="M15:S15"/>
-    <mergeCell ref="T15:Z15"/>
-    <mergeCell ref="AA15:AG15"/>
-    <mergeCell ref="AJ15:AY15"/>
-    <mergeCell ref="M16:S16"/>
-    <mergeCell ref="T16:Z16"/>
-    <mergeCell ref="AA16:AG16"/>
-    <mergeCell ref="AH16:AI16"/>
-    <mergeCell ref="AJ16:AY16"/>
-    <mergeCell ref="AH15:AI15"/>
-    <mergeCell ref="F17:L17"/>
-    <mergeCell ref="F18:L18"/>
-    <mergeCell ref="M17:S17"/>
-    <mergeCell ref="T17:Z17"/>
-    <mergeCell ref="AA17:AG17"/>
-    <mergeCell ref="AJ17:AY17"/>
-    <mergeCell ref="M18:S18"/>
-    <mergeCell ref="T18:Z18"/>
-    <mergeCell ref="AA18:AG18"/>
-    <mergeCell ref="AH18:AI18"/>
-    <mergeCell ref="AJ18:AY18"/>
-    <mergeCell ref="AH17:AI17"/>
-    <mergeCell ref="F21:L21"/>
-    <mergeCell ref="F22:L22"/>
-    <mergeCell ref="F19:L19"/>
-    <mergeCell ref="F20:L20"/>
-    <mergeCell ref="M19:S19"/>
-    <mergeCell ref="AJ19:AY19"/>
-    <mergeCell ref="M20:S20"/>
-    <mergeCell ref="T20:Z20"/>
-    <mergeCell ref="AA20:AG20"/>
-    <mergeCell ref="AH20:AI20"/>
-    <mergeCell ref="AJ20:AY20"/>
-    <mergeCell ref="T19:Z19"/>
-    <mergeCell ref="AA19:AG19"/>
-    <mergeCell ref="AH19:AI19"/>
-    <mergeCell ref="AJ21:AY21"/>
-    <mergeCell ref="M22:S22"/>
-    <mergeCell ref="T22:Z22"/>
-    <mergeCell ref="AA22:AG22"/>
-    <mergeCell ref="AH22:AI22"/>
-    <mergeCell ref="AJ22:AY22"/>
-    <mergeCell ref="M21:S21"/>
-    <mergeCell ref="T21:Z21"/>
-    <mergeCell ref="AA21:AG21"/>
-    <mergeCell ref="AH21:AI21"/>
-    <mergeCell ref="AH9:AI9"/>
-    <mergeCell ref="AJ9:AY9"/>
-    <mergeCell ref="F9:L9"/>
-    <mergeCell ref="M9:S9"/>
-    <mergeCell ref="T9:Z9"/>
-    <mergeCell ref="AA9:AG9"/>
+    <mergeCell ref="F11:L11"/>
+    <mergeCell ref="F12:L12"/>
+    <mergeCell ref="M11:S11"/>
+    <mergeCell ref="T11:Z11"/>
+    <mergeCell ref="AA11:AG11"/>
+    <mergeCell ref="AJ10:AY10"/>
+    <mergeCell ref="F10:L10"/>
+    <mergeCell ref="M10:S10"/>
+    <mergeCell ref="T10:Z10"/>
+    <mergeCell ref="AA10:AG10"/>
+    <mergeCell ref="AH10:AI10"/>
   </mergeCells>
-  <phoneticPr fontId="4"/>
+  <phoneticPr fontId="5"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH9:AI22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH9:AI18">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>